<commit_message>
chore: update listName.xlsx and remove temporary file ~$listName.xlsx
</commit_message>
<xml_diff>
--- a/listName.xlsx
+++ b/listName.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanpetchboriboon/Repository/Workspace/random-name/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4AE42519-A7E4-BF4F-9984-7A06B2131B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{41BB5292-F712-B54B-B03C-AE65643549B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="660" windowWidth="28040" windowHeight="17160" xr2:uid="{E5FEB766-AA2C-B64E-9FFA-C56EF69A4BF6}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="59">
   <si>
     <t>รายชื่อ</t>
   </si>
@@ -179,6 +179,24 @@
   </si>
   <si>
     <t>กุลชญา</t>
+  </si>
+  <si>
+    <t>สมบูรณ์</t>
+  </si>
+  <si>
+    <t>ปิยมาภรณ์</t>
+  </si>
+  <si>
+    <t>รู้นันต๊ะ</t>
+  </si>
+  <si>
+    <t>พี่มี่</t>
+  </si>
+  <si>
+    <t>ทัศน์พล</t>
+  </si>
+  <si>
+    <t>ผดุงโกเม็ด</t>
   </si>
 </sst>
 </file>
@@ -1047,10 +1065,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{902EFBE2-80A3-0C4C-8632-72EB648BE2AD}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1166,6 +1184,12 @@
       <c r="A14" t="s">
         <v>13</v>
       </c>
+      <c r="B14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -1302,6 +1326,12 @@
       <c r="A28" t="s">
         <v>26</v>
       </c>
+      <c r="B28" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
@@ -1312,6 +1342,17 @@
       </c>
       <c r="C29" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>